<commit_message>
as on 30th june
</commit_message>
<xml_diff>
--- a/7Rmart/src/test/resources/testdata.xlsx
+++ b/7Rmart/src/test/resources/testdata.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40742F5-6E02-430F-9095-EE421C0C8506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3CA216-2B97-463E-A00A-C0495DB08028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{EE47C0D1-B5E4-4E63-B1F0-82DA7EF78E6C}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{EE47C0D1-B5E4-4E63-B1F0-82DA7EF78E6C}"/>
   </bookViews>
   <sheets>
     <sheet name="loginpage" sheetId="1" r:id="rId1"/>
     <sheet name="managenews" sheetId="2" r:id="rId2"/>
-    <sheet name="managecontact" sheetId="3" r:id="rId3"/>
-    <sheet name="managecategory" sheetId="4" r:id="rId4"/>
+    <sheet name="adminuser" sheetId="5" r:id="rId3"/>
+    <sheet name="managecontact" sheetId="3" r:id="rId4"/>
+    <sheet name="managecategory" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -82,6 +83,15 @@
   </si>
   <si>
     <t>Sample</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>Ezabella</t>
+  </si>
+  <si>
+    <t>ezabella</t>
   </si>
 </sst>
 </file>
@@ -502,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C42F08B-1C82-42EF-821D-EB5EB694A756}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -524,6 +534,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28901E9-00CB-48B3-B4F3-A080EE754A4B}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2696D7-1BA7-4BE9-A055-0B84DD138BFB}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -577,7 +617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D234D4-1C78-41C5-9241-DD7472EFA4F9}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>